<commit_message>
First two druid subclasses completed
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Archetypes/Druid.xlsx
+++ b/CoreRulebook/Data/Archetypes/Druid.xlsx
@@ -91,6 +91,9 @@
     <t xml:space="preserve">Disciplines:</t>
   </si>
   <si>
+    <t xml:space="preserve">Choose 3 from Elemental, Telepathy, Bewitchment, Healing, Warding and Alteration. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Aspect Feature III</t>
   </si>
   <si>
@@ -136,7 +139,7 @@
     <t xml:space="preserve">List2 Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Ancient Knowledge</t>
+    <t xml:space="preserve">Ancient Powers</t>
   </si>
   <si>
     <t xml:space="preserve">Master</t>
@@ -146,9 +149,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nature Affinity III</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aspect Feature VI</t>
   </si>
   <si>
     <t xml:space="preserve">Ascendant</t>
@@ -285,7 +285,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -425,7 +425,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -442,6 +442,9 @@
       <c r="G7" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="H7" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -455,10 +458,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>17</v>
@@ -473,13 +476,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,16 +494,16 @@
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,16 +515,16 @@
         <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,13 +536,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,10 +554,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -566,10 +569,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,7 +584,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,10 +596,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,7 +611,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,10 +623,10 @@
         <v>6</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,10 +638,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>